<commit_message>
-- Fetch Payment Status feature
</commit_message>
<xml_diff>
--- a/Database/sheet.xlsx
+++ b/Database/sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="1">
   <si>
     <t>PAID</t>
   </si>
@@ -376,7 +376,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
       <c r="F10" t="s">
         <v>0</v>
       </c>

</xml_diff>